<commit_message>
Added bulk email template
</commit_message>
<xml_diff>
--- a/Epi.Web/Content/Text/EmailList-Bulk.xlsx
+++ b/Epi.Web/Content/Text/EmailList-Bulk.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vwm5\source\repos\Epi-Info\Epi-Info-Web-Survey\Epi.Web\Content\Text\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCBABE96-F9E7-43C5-94D2-37AE6DF9D3CF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D40FE7DD-1F27-4721-8559-8479E2B1DD43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,9 +34,6 @@
     <t xml:space="preserve">ResponseId </t>
   </si>
   <si>
-    <t>vwm5@cdc.gov</t>
-  </si>
-  <si>
     <t>Response Status</t>
   </si>
   <si>
@@ -106,7 +103,10 @@
     <t>Email body for the initial email.</t>
   </si>
   <si>
-    <t>epiinfo@cdc.gov</t>
+    <t>EmailAddress@email.com</t>
+  </si>
+  <si>
+    <t>Sender@senderemail.com</t>
   </si>
 </sst>
 </file>
@@ -551,15 +551,15 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.85546875" customWidth="1"/>
-    <col min="2" max="2" width="22" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" style="2" customWidth="1"/>
     <col min="5" max="5" width="24" style="2" customWidth="1"/>
     <col min="6" max="6" width="52.5703125" style="2" customWidth="1"/>
     <col min="7" max="7" width="9.140625" style="3"/>
@@ -570,34 +570,34 @@
   <sheetData>
     <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>8</v>
-      </c>
       <c r="J1" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -605,28 +605,28 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="J3" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
       <c r="J4" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="J5" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -645,7 +645,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C2" sqref="C2:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -658,50 +658,50 @@
   <sheetData>
     <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="C1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>5</v>
-      </c>
       <c r="D1" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>23</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>24</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>11</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{21C7F2F9-A024-4568-96D7-79E8F0F4FC64}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>